<commit_message>
Solving the slideshow images problem
</commit_message>
<xml_diff>
--- a/Solina/Consumption/Results_Consumption.xlsx
+++ b/Solina/Consumption/Results_Consumption.xlsx
@@ -23,6 +23,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -52,8 +55,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A145"/>
+  <dimension ref="A1:A95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,723 +364,473 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2">
-        <v>0.09589425474405289</v>
+      <c r="A2" s="1">
+        <v>0.1850714385509491</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3">
-        <v>0.09318127483129501</v>
+      <c r="A3" s="1">
+        <v>0.1760987341403961</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
-        <v>0.08918378502130508</v>
+      <c r="A4" s="1">
+        <v>0.1706276088953018</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5">
-        <v>0.08925148844718933</v>
+      <c r="A5" s="1">
+        <v>0.1613334566354752</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6">
-        <v>0.0858452171087265</v>
+      <c r="A6" s="1">
+        <v>0.155338242650032</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7">
-        <v>0.08972515165805817</v>
+      <c r="A7" s="1">
+        <v>0.1595547795295715</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8">
-        <v>0.1113284379243851</v>
+      <c r="A8" s="1">
+        <v>0.1463826298713684</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9">
-        <v>0.1567369699478149</v>
+      <c r="A9" s="1">
+        <v>0.1348744779825211</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10">
-        <v>0.1865218579769135</v>
+      <c r="A10" s="1">
+        <v>0.1315028518438339</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11">
-        <v>0.2074995636940002</v>
+      <c r="A11" s="1">
+        <v>0.1362364143133163</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12">
-        <v>0.216718316078186</v>
+      <c r="A12" s="1">
+        <v>0.1349645256996155</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13">
-        <v>0.2054769545793533</v>
+      <c r="A13" s="1">
+        <v>0.130864679813385</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14">
-        <v>0.2164687365293503</v>
+      <c r="A14" s="1">
+        <v>0.1125651821494102</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15">
-        <v>0.2140318006277084</v>
+      <c r="A15" s="1">
+        <v>0.09689251333475113</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16">
-        <v>0.2091182470321655</v>
+      <c r="A16" s="1">
+        <v>0.09291697293519974</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17">
-        <v>0.1969312876462936</v>
+      <c r="A17" s="1">
+        <v>0.09080435335636139</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18">
-        <v>0.1934086978435516</v>
+      <c r="A18" s="1">
+        <v>0.08793919533491135</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19">
-        <v>0.1660820245742798</v>
+      <c r="A19" s="1">
+        <v>0.08260254561901093</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20">
-        <v>0.1541871577501297</v>
+      <c r="A20" s="1">
+        <v>0.08349675685167313</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21">
-        <v>0.1533399075269699</v>
+      <c r="A21" s="1">
+        <v>0.08843749761581421</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22">
-        <v>0.1536990404129028</v>
+      <c r="A22" s="1">
+        <v>0.09150766581296921</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23">
-        <v>0.1514032483100891</v>
+      <c r="A23" s="1">
+        <v>0.08189771324396133</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24">
-        <v>0.1376140266656876</v>
+      <c r="A24" s="1">
+        <v>0.08357468247413635</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25">
-        <v>0.1175383925437927</v>
+      <c r="A25" s="1">
+        <v>0.08185264468193054</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26">
-        <v>0.09615853428840637</v>
+      <c r="A26" s="1">
+        <v>0.07764860242605209</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27">
-        <v>0.09213433414697647</v>
+      <c r="A27" s="1">
+        <v>0.07497376948595047</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28">
-        <v>0.08813684433698654</v>
+      <c r="A28" s="1">
+        <v>0.07074220478534698</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29">
-        <v>0.08672186732292175</v>
+      <c r="A29" s="1">
+        <v>0.06769091635942459</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30">
-        <v>0.08678093552589417</v>
+      <c r="A30" s="1">
+        <v>0.07216963917016983</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31">
-        <v>0.09174569696187973</v>
+      <c r="A31" s="1">
+        <v>0.07652962207794189</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32">
-        <v>0.1124850884079933</v>
+      <c r="A32" s="1">
+        <v>0.07438062876462936</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33">
-        <v>0.1584126800298691</v>
+      <c r="A33" s="1">
+        <v>0.0735531821846962</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34">
-        <v>0.1922005116939545</v>
+      <c r="A34" s="1">
+        <v>0.07222521305084229</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35">
-        <v>0.2099202573299408</v>
+      <c r="A35" s="1">
+        <v>0.0738646388053894</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36">
-        <v>0.2165777683258057</v>
+      <c r="A36" s="1">
+        <v>0.07428913563489914</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37">
-        <v>0.202093318104744</v>
+      <c r="A37" s="1">
+        <v>0.07330787926912308</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38">
-        <v>0.2135128378868103</v>
+      <c r="A38" s="1">
+        <v>0.07463182508945465</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39">
-        <v>0.209384873509407</v>
+      <c r="A39" s="1">
+        <v>0.0713663175702095</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40">
-        <v>0.2054274082183838</v>
+      <c r="A40" s="1">
+        <v>0.0872621014714241</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41">
-        <v>0.1939719617366791</v>
+      <c r="A41" s="1">
+        <v>0.08274365961551666</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42">
-        <v>0.1865279376506805</v>
+      <c r="A42" s="1">
+        <v>0.08110301196575165</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43">
-        <v>0.1760257333517075</v>
+      <c r="A43" s="1">
+        <v>0.08000288903713226</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44">
-        <v>0.1696114391088486</v>
+      <c r="A44" s="1">
+        <v>0.08034301549196243</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45">
-        <v>0.174544021487236</v>
+      <c r="A45" s="1">
+        <v>0.08447057753801346</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46">
-        <v>0.1707886904478073</v>
+      <c r="A46" s="1">
+        <v>0.08289280533790588</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47">
-        <v>0.1730679124593735</v>
+      <c r="A47" s="1">
+        <v>0.07435993105173111</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48">
-        <v>0.1585813462734222</v>
+      <c r="A48" s="1">
+        <v>0.07374291121959686</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49">
-        <v>0.1334594786167145</v>
+      <c r="A49" s="1">
+        <v>0.07257001847028732</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50">
-        <v>0.1038332134485245</v>
+      <c r="A50" s="1">
+        <v>0.1706276088953018</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51">
-        <v>0.09928524494171143</v>
+      <c r="A51" s="1">
+        <v>0.1613334566354752</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52">
-        <v>0.1009510159492493</v>
+      <c r="A52" s="1">
+        <v>0.155338242650032</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53">
-        <v>0.09803689271211624</v>
+      <c r="A53" s="1">
+        <v>0.1595547795295715</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54">
-        <v>0.1007320284843445</v>
+      <c r="A54" s="1">
+        <v>0.1463826298713684</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55">
-        <v>0.1093324348330498</v>
+      <c r="A55" s="1">
+        <v>0.1348744779825211</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56">
-        <v>0.1379338353872299</v>
+      <c r="A56" s="1">
+        <v>0.1315028518438339</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57">
-        <v>0.1722738146781921</v>
+      <c r="A57" s="1">
+        <v>0.1362364143133163</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58">
-        <v>0.1954204887151718</v>
+      <c r="A58" s="1">
+        <v>0.1349645256996155</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59">
-        <v>0.2056718319654465</v>
+      <c r="A59" s="1">
+        <v>0.130864679813385</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60">
-        <v>0.2222418189048767</v>
+      <c r="A60" s="1">
+        <v>0.1125651821494102</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61">
-        <v>0.2217562794685364</v>
+      <c r="A61" s="1">
+        <v>0.09689251333475113</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62">
-        <v>0.2091365605592728</v>
+      <c r="A62" s="1">
+        <v>0.09291697293519974</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63">
-        <v>0.1867259740829468</v>
+      <c r="A63" s="1">
+        <v>0.09080435335636139</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64">
-        <v>0.1911800354719162</v>
+      <c r="A64" s="1">
+        <v>0.08793919533491135</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65">
-        <v>0.1781941652297974</v>
+      <c r="A65" s="1">
+        <v>0.08260254561901093</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66">
-        <v>0.1635516434907913</v>
+      <c r="A66" s="1">
+        <v>0.08349675685167313</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67">
-        <v>0.1563405096530914</v>
+      <c r="A67" s="1">
+        <v>0.08843749761581421</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68">
-        <v>0.1422145068645477</v>
+      <c r="A68" s="1">
+        <v>0.09150766581296921</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69">
-        <v>0.1477005928754807</v>
+      <c r="A69" s="1">
+        <v>0.08189771324396133</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70">
-        <v>0.1508063226938248</v>
+      <c r="A70" s="1">
+        <v>0.08357468247413635</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71">
-        <v>0.1492389589548111</v>
+      <c r="A71" s="1">
+        <v>0.08185264468193054</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72">
-        <v>0.1400406360626221</v>
+      <c r="A72" s="1">
+        <v>0.07764860242605209</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73">
-        <v>0.1264598220586777</v>
+      <c r="A73" s="1">
+        <v>0.07497376948595047</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74">
-        <v>0.1010246202349663</v>
+      <c r="A74" s="1">
+        <v>0.07074220478534698</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75">
-        <v>0.1000592708587646</v>
+      <c r="A75" s="1">
+        <v>0.06769091635942459</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76">
-        <v>0.09981641918420792</v>
+      <c r="A76" s="1">
+        <v>0.07216963917016983</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77">
-        <v>0.1002595648169518</v>
+      <c r="A77" s="1">
+        <v>0.07652962207794189</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78">
-        <v>0.09545668214559555</v>
+      <c r="A78" s="1">
+        <v>0.07438062876462936</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79">
-        <v>0.1000718027353287</v>
+      <c r="A79" s="1">
+        <v>0.0735531821846962</v>
       </c>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80">
-        <v>0.103732742369175</v>
+      <c r="A80" s="1">
+        <v>0.07222521305084229</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81">
-        <v>0.1094320490956306</v>
+      <c r="A81" s="1">
+        <v>0.0738646388053894</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82">
-        <v>0.1115080937743187</v>
+      <c r="A82" s="1">
+        <v>0.07428913563489914</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83">
-        <v>0.116859070956707</v>
+      <c r="A83" s="1">
+        <v>0.07330787926912308</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84">
-        <v>0.1141335070133209</v>
+      <c r="A84" s="1">
+        <v>0.07463182508945465</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85">
-        <v>0.1234640777111053</v>
+      <c r="A85" s="1">
+        <v>0.0713663175702095</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86">
-        <v>0.1385092288255692</v>
+      <c r="A86" s="1">
+        <v>0.0872621014714241</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87">
-        <v>0.1205909326672554</v>
+      <c r="A87" s="1">
+        <v>0.08274365961551666</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88">
-        <v>0.1191204339265823</v>
+      <c r="A88" s="1">
+        <v>0.08110301196575165</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89">
-        <v>0.1019021049141884</v>
+      <c r="A89" s="1">
+        <v>0.08000288903713226</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90">
-        <v>0.07823049277067184</v>
+      <c r="A90" s="1">
+        <v>0.08034301549196243</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91">
-        <v>0.07533793896436691</v>
+      <c r="A91" s="1">
+        <v>0.08447057753801346</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92">
-        <v>0.07949591428041458</v>
+      <c r="A92" s="1">
+        <v>0.08289280533790588</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93">
-        <v>0.08209703117609024</v>
+      <c r="A93" s="1">
+        <v>0.07435993105173111</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94">
-        <v>0.08129604160785675</v>
+      <c r="A94" s="1">
+        <v>0.07374291121959686</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95">
-        <v>0.0822511613368988</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96">
-        <v>0.08115100115537643</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97">
-        <v>0.08124850690364838</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98">
-        <v>0.08697126805782318</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99">
-        <v>0.08514824509620667</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100">
-        <v>0.08514824509620667</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101">
-        <v>0.0855913907289505</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102">
-        <v>0.08652713894844055</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103">
-        <v>0.08590690791606903</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104">
-        <v>0.08778949081897736</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105">
-        <v>0.09067171812057495</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106">
-        <v>0.09002023935317993</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107">
-        <v>0.08856692910194397</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108">
-        <v>0.09354975074529648</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109">
-        <v>0.09225268661975861</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110">
-        <v>0.08847705274820328</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111">
-        <v>0.09697888046503067</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112">
-        <v>0.1017154008150101</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113">
-        <v>0.08893608301877975</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114">
-        <v>0.07983110845088959</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115">
-        <v>0.07930172234773636</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116">
-        <v>0.07324972003698349</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117">
-        <v>0.07800503075122833</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118">
-        <v>0.08281885832548141</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119">
-        <v>0.0801113024353981</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120">
-        <v>0.07952576875686646</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121">
-        <v>0.07937731593847275</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
-      <c r="A122">
-        <v>0.1029611304402351</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123">
-        <v>0.09781605005264282</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1">
-      <c r="A124">
-        <v>0.1018318682909012</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1">
-      <c r="A125">
-        <v>0.1016418561339378</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126">
-        <v>0.09188224375247955</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127">
-        <v>0.1025096401572227</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128">
-        <v>0.1406237781047821</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129">
-        <v>0.1806354224681854</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
-      <c r="A130">
-        <v>0.22573022544384</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131">
-        <v>0.2379094213247299</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132">
-        <v>0.2390861213207245</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133">
-        <v>0.2222016751766205</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1">
-      <c r="A134">
-        <v>0.2138346284627914</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1">
-      <c r="A135">
-        <v>0.2100949734449387</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1">
-      <c r="A136">
-        <v>0.2035586535930634</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1">
-      <c r="A137">
-        <v>0.2020866721868515</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1">
-      <c r="A138">
-        <v>0.1911580413579941</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
-      <c r="A139">
-        <v>0.1735057681798935</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1">
-      <c r="A140">
-        <v>0.1709852665662766</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1">
-      <c r="A141">
-        <v>0.1791878640651703</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1">
-      <c r="A142">
-        <v>0.1840893179178238</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1">
-      <c r="A143">
-        <v>0.1856202632188797</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1">
-      <c r="A144">
-        <v>0.175346776843071</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1">
-      <c r="A145">
-        <v>0.1474990844726562</v>
+      <c r="A95" s="1">
+        <v>0.07257001847028732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automating the Solina and RAAL consumptions
</commit_message>
<xml_diff>
--- a/Solina/Consumption/Results_Consumption.xlsx
+++ b/Solina/Consumption/Results_Consumption.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A95"/>
+  <dimension ref="A1:A156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,472 +365,777 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1">
-        <v>0.1850714385509491</v>
+        <v>0.1056026443839073</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1">
-        <v>0.1760987341403961</v>
+        <v>0.09806323796510696</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1">
-        <v>0.1706276088953018</v>
+        <v>0.09596473723649979</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1">
-        <v>0.1613334566354752</v>
+        <v>0.09087328612804413</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1">
-        <v>0.155338242650032</v>
+        <v>0.09317360073328018</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1">
-        <v>0.1595547795295715</v>
+        <v>0.1015491411089897</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1">
-        <v>0.1463826298713684</v>
+        <v>0.1451462507247925</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1">
-        <v>0.1348744779825211</v>
+        <v>0.1764229983091354</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1">
-        <v>0.1315028518438339</v>
+        <v>0.1978478878736496</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1">
-        <v>0.1362364143133163</v>
+        <v>0.1990372389554977</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1">
-        <v>0.1349645256996155</v>
+        <v>0.1978534013032913</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1">
-        <v>0.130864679813385</v>
+        <v>0.1886269897222519</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1">
-        <v>0.1125651821494102</v>
+        <v>0.1854834705591202</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1">
-        <v>0.09689251333475113</v>
+        <v>0.1762103885412216</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1">
-        <v>0.09291697293519974</v>
+        <v>0.1636193096637726</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1">
-        <v>0.09080435335636139</v>
+        <v>0.162919819355011</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1">
-        <v>0.08793919533491135</v>
+        <v>0.152069017291069</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1">
-        <v>0.08260254561901093</v>
+        <v>0.1397820264101028</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1">
-        <v>0.08349675685167313</v>
+        <v>0.1369117349386215</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1">
-        <v>0.08843749761581421</v>
+        <v>0.1410485506057739</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1">
-        <v>0.09150766581296921</v>
+        <v>0.1395169049501419</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1">
-        <v>0.08189771324396133</v>
+        <v>0.1311882734298706</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1">
-        <v>0.08357468247413635</v>
+        <v>0.1133195608854294</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1">
-        <v>0.08185264468193054</v>
+        <v>0.1062970608472824</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1">
-        <v>0.07764860242605209</v>
+        <v>0.0944255068898201</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1">
-        <v>0.07497376948595047</v>
+        <v>0.08999232947826385</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1">
-        <v>0.07074220478534698</v>
+        <v>0.08739485591650009</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1">
-        <v>0.06769091635942459</v>
+        <v>0.08625379949808121</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1">
-        <v>0.07216963917016983</v>
+        <v>0.08714801073074341</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1">
-        <v>0.07652962207794189</v>
+        <v>0.09049210697412491</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1">
-        <v>0.07438062876462936</v>
+        <v>0.09036631137132645</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1">
-        <v>0.0735531821846962</v>
+        <v>0.08960402756929398</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1">
-        <v>0.07222521305084229</v>
+        <v>0.08972924947738647</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1">
-        <v>0.0738646388053894</v>
+        <v>0.08797987550497055</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1">
-        <v>0.07428913563489914</v>
+        <v>0.08824003487825394</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1">
-        <v>0.07330787926912308</v>
+        <v>0.08589421957731247</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1">
-        <v>0.07463182508945465</v>
+        <v>0.08397543430328369</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1">
-        <v>0.0713663175702095</v>
+        <v>0.08113499730825424</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1">
-        <v>0.0872621014714241</v>
+        <v>0.07932413369417191</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1">
-        <v>0.08274365961551666</v>
+        <v>0.07689343392848969</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1">
-        <v>0.08110301196575165</v>
+        <v>0.07447367906570435</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1">
-        <v>0.08000288903713226</v>
+        <v>0.07485280185937881</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="1">
-        <v>0.08034301549196243</v>
+        <v>0.07302823662757874</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1">
-        <v>0.08447057753801346</v>
+        <v>0.07566092908382416</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="1">
-        <v>0.08289280533790588</v>
+        <v>0.07618246227502823</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1">
-        <v>0.07435993105173111</v>
+        <v>0.07336227595806122</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="1">
-        <v>0.07374291121959686</v>
+        <v>0.07110990583896637</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1">
-        <v>0.07257001847028732</v>
+        <v>0.07004912942647934</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1">
-        <v>0.1706276088953018</v>
+        <v>0.08768191188573837</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1">
-        <v>0.1613334566354752</v>
+        <v>0.08452703058719635</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1">
-        <v>0.155338242650032</v>
+        <v>0.08288638293743134</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="1">
-        <v>0.1595547795295715</v>
+        <v>0.08208984136581421</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1">
-        <v>0.1463826298713684</v>
+        <v>0.08298405259847641</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1">
-        <v>0.1348744779825211</v>
+        <v>0.08703645318746567</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="1">
-        <v>0.1315028518438339</v>
+        <v>0.08487524092197418</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="1">
-        <v>0.1362364143133163</v>
+        <v>0.0821402370929718</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1">
-        <v>0.1349645256996155</v>
+        <v>0.08285330981016159</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="1">
-        <v>0.130864679813385</v>
+        <v>0.08223347365856171</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="1">
-        <v>0.1125651821494102</v>
+        <v>0.08016877621412277</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="1">
-        <v>0.09689251333475113</v>
+        <v>0.07626821845769882</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1">
-        <v>0.09291697293519974</v>
+        <v>0.07129251956939697</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="1">
-        <v>0.09080435335636139</v>
+        <v>0.07426422834396362</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1">
-        <v>0.08793919533491135</v>
+        <v>0.07452625781297684</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="1">
-        <v>0.08260254561901093</v>
+        <v>0.07611998915672302</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1">
-        <v>0.08349675685167313</v>
+        <v>0.07241465151309967</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="1">
-        <v>0.08843749761581421</v>
+        <v>0.07692595571279526</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1">
-        <v>0.09150766581296921</v>
+        <v>0.07759345322847366</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="1">
-        <v>0.08189771324396133</v>
+        <v>0.08485069125890732</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1">
-        <v>0.08357468247413635</v>
+        <v>0.08583956211805344</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="1">
-        <v>0.08185264468193054</v>
+        <v>0.08014824986457825</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="1">
-        <v>0.07764860242605209</v>
+        <v>0.07356823980808258</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="1">
-        <v>0.07497376948595047</v>
+        <v>0.07434379309415817</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="1">
-        <v>0.07074220478534698</v>
+        <v>0.0879397988319397</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="1">
-        <v>0.06769091635942459</v>
+        <v>0.08594207465648651</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="1">
-        <v>0.07216963917016983</v>
+        <v>0.08859008550643921</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="1">
-        <v>0.07652962207794189</v>
+        <v>0.08848121017217636</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="1">
-        <v>0.07438062876462936</v>
+        <v>0.08726364374160767</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="1">
-        <v>0.0735531821846962</v>
+        <v>0.0948173776268959</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="1">
-        <v>0.07222521305084229</v>
+        <v>0.1319430023431778</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="1">
-        <v>0.0738646388053894</v>
+        <v>0.1777654439210892</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="1">
-        <v>0.07428913563489914</v>
+        <v>0.2061997503042221</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="1">
-        <v>0.07330787926912308</v>
+        <v>0.2222494632005692</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="1">
-        <v>0.07463182508945465</v>
+        <v>0.2104895412921906</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="1">
-        <v>0.0713663175702095</v>
+        <v>0.2053017914295197</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="1">
-        <v>0.0872621014714241</v>
+        <v>0.2013587802648544</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="1">
-        <v>0.08274365961551666</v>
+        <v>0.1938804686069489</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="1">
-        <v>0.08110301196575165</v>
+        <v>0.1848463267087936</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="1">
-        <v>0.08000288903713226</v>
+        <v>0.1858280748128891</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1">
-        <v>0.08034301549196243</v>
+        <v>0.1699197292327881</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1">
-        <v>0.08447057753801346</v>
+        <v>0.1678435504436493</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="1">
-        <v>0.08289280533790588</v>
+        <v>0.1636290103197098</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1">
-        <v>0.07435993105173111</v>
+        <v>0.1648920774459839</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="1">
-        <v>0.07374291121959686</v>
+        <v>0.1667213886976242</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1">
-        <v>0.07257001847028732</v>
+        <v>0.1615720093250275</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="1">
+        <v>0.1247084885835648</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="1">
+        <v>0.1073317229747772</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="1">
+        <v>0.1046975776553154</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="1">
+        <v>0.09925060719251633</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="1">
+        <v>0.1045616045594215</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="1">
+        <v>0.1037989035248756</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="1">
+        <v>0.09332532435655594</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="1">
+        <v>0.1003702506422997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="1">
+        <v>0.1444872915744781</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="1">
+        <v>0.1839158833026886</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="1">
+        <v>0.2095482051372528</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="1">
+        <v>0.2254806011915207</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="1">
+        <v>0.2193359732627869</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="1">
+        <v>0.2065916657447815</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="1">
+        <v>0.2056795954704285</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="1">
+        <v>0.1968738734722137</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1">
+        <v>0.1876902282238007</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1">
+        <v>0.1876541525125504</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="1">
+        <v>0.1775341182947159</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="1">
+        <v>0.1671268790960312</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="1">
+        <v>0.1628993004560471</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="1">
+        <v>0.1719160526990891</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="1">
+        <v>0.168288066983223</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="1">
+        <v>0.1682065725326538</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="1">
+        <v>0.1454377472400665</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="1">
+        <v>0.1245240643620491</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="1">
+        <v>0.1087479367852211</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="1">
+        <v>0.1011644825339317</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="1">
+        <v>0.09873849898576736</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="1">
+        <v>0.09690376371145248</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="1">
+        <v>0.0977586954832077</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="1">
+        <v>0.1050778105854988</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="1">
+        <v>0.1460853666067123</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="1">
+        <v>0.1909648329019547</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="1">
+        <v>0.2153187543153763</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="1">
+        <v>0.220765620470047</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="1">
+        <v>0.220290794968605</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="1">
+        <v>0.2097830921411514</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="1">
+        <v>0.2113891690969467</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="1">
+        <v>0.202499195933342</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="1">
+        <v>0.1886700540781021</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="1">
+        <v>0.1873032301664352</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="1">
+        <v>0.177996352314949</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="1">
+        <v>0.1672581732273102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="1">
+        <v>0.1639053523540497</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="1">
+        <v>0.1671480089426041</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="1">
+        <v>0.1664849519729614</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="1">
+        <v>0.1615317910909653</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="1">
+        <v>0.1355683654546738</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="1">
+        <v>0.115163654088974</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="1">
+        <v>0.1091917157173157</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="1">
+        <v>0.1016082614660263</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="1">
+        <v>0.09950978308916092</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="1">
+        <v>0.09830059856176376</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="1">
+        <v>0.09899407625198364</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="1">
+        <v>0.1082462519407272</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="1">
+        <v>0.1490663141012192</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="1">
+        <v>0.1841649115085602</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="1">
+        <v>0.2147525697946548</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="1">
+        <v>0.2201407104730606</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="1">
+        <v>0.2224241495132446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>